<commit_message>
image scraper first try
</commit_message>
<xml_diff>
--- a/scraped_data_test.xlsx
+++ b/scraped_data_test.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>One</t>
+    <t>OneOneOneOne</t>
   </si>
   <si>
     <t>Two</t>
@@ -58,8 +58,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +432,7 @@
       </c>
     </row>
     <row r="5" ht="70" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>